<commit_message>
paul mking it publishable
</commit_message>
<xml_diff>
--- a/uploaded_folder/file_VKDS_1.xlsx
+++ b/uploaded_folder/file_VKDS_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skfgroup-my.sharepoint.com/personal/sanjai_b_skf_com/Documents/Desktop/py/motor_app/input_folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkeck/localdocs/SKF/extractionapp/uploaded_folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35C315D3-D61D-44E0-9880-7D28F4406ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2067D0F-F298-DC49-9E0B-A8B6EE9412C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C0D95AE5-656D-4938-A3CF-B54468D13BFD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{C0D95AE5-656D-4938-A3CF-B54468D13BFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,48 +416,38 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A7" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>12552954</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>12556582</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>12552953</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>12360440</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>381263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>382880</v>
-      </c>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>